<commit_message>
Made required changes to Sports output file
</commit_message>
<xml_diff>
--- a/Archery_final.xlsx
+++ b/Archery_final.xlsx
@@ -382,12 +382,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -399,12 +399,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -416,12 +416,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_boys</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Archery-Boys</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -433,12 +433,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_girls</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Archery-Girls</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -450,12 +450,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -467,12 +467,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -484,12 +484,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -501,12 +501,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>
@@ -518,12 +518,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>club-sports</t>
+          <t>sports_club_coed</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Archery-Coed</t>
+          <t>Archery</t>
         </is>
       </c>
     </row>

</xml_diff>